<commit_message>
New tests and code
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/SAEVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B082815-2920-B74D-984B-60892DBB5DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1DA6A5-685D-1047-BCAD-D01CE7020B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$102</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +82,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,13 +124,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,6 +149,1147 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total demand</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>239.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>239.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>239.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>239.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>796.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>796.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>796.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>796.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3524</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3524</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3524</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3524</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12460.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12460.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12460.25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12460.25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33464.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33464.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33464.25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33464.25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>66297</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66297</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>66297</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>66297</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>52173</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>52173</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>52173</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>52173</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17376.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17376.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17376.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17376.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7898</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7898</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7898</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7898</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5980.25</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5980.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5980.25</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5980.25</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>25595</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25595</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>25595</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>25595</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>26476</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>26476</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>26476</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>26476</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>30789.25</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>30789.25</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>30789.25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>30789.25</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44572.75</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>44572.75</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>44572.75</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>44572.75</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>56643</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>56643</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>56643</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>56643</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>49975.25</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>49975.25</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>49975.25</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>49975.25</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>32104</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>32104</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>32104</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>32104</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>22266.75</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>22266.75</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>22266.75</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>22266.75</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>16930.5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>16930.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>16930.5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>16930.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>13005.25</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>13005.25</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13005.25</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>13005.25</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8475</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8475</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8475</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8475</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4897</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4897</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4897</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A431-3643-B601-2A82B82E6529}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1730397472"/>
+        <c:axId val="1730399184"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1730397472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1730399184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1730399184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1730397472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57C2C3A-81E6-3CBA-7455-B816A3ABE7F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99:G102"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,21 +1612,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>41.5</v>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>50.5</v>
       </c>
       <c r="B2">
         <f>ROUND(A2*0.01,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>ROUND(A2*0.05,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <f>ROUND(A2*0.1,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <f>0*$F$2</f>
@@ -484,72 +1637,72 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>41.5</v>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>50.5</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" si="0">ROUND(A3*0.01,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="1">ROUND(A3*0.05,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" si="2">ROUND(A3*0.1,0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <f>0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>41.5</v>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>50.5</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <f>0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>41.5</v>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>50.5</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <f>5*$F$2</f>
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>100</v>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>112.5</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -557,20 +1710,20 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <f>5*$F$2</f>
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>100</v>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>112.5</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -578,20 +1731,20 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <f>6*$F$2</f>
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>100</v>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>112.5</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -599,20 +1752,20 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <f>6*$F$2</f>
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>100</v>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>112.5</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -620,20 +1773,20 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <f>10*$F$2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>235.75</v>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>239.25</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -652,9 +1805,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>235.75</v>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>239.25</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -673,9 +1826,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>235.75</v>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>239.25</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -694,9 +1847,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>235.75</v>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>239.25</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -715,9 +1868,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>755.25</v>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>796.5</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -725,20 +1878,20 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E14">
         <f>1*$F$2</f>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>755.25</v>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>796.5</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -746,20 +1899,20 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E15">
         <f t="shared" ref="E15:E21" si="4">0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>755.25</v>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>796.5</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -767,20 +1920,20 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>755.25</v>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>796.5</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -788,1691 +1941,1691 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>2460.25</v>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>3524</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>246</v>
+        <v>352</v>
       </c>
       <c r="E18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2460.25</v>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>3524</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>246</v>
+        <v>352</v>
       </c>
       <c r="E19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>2460.25</v>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>3524</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>246</v>
+        <v>352</v>
       </c>
       <c r="E20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>2460.25</v>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>3524</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="D21">
         <f t="shared" si="2"/>
-        <v>246</v>
+        <v>352</v>
       </c>
       <c r="E21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>5302.25</v>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>12460.25</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>623</v>
       </c>
       <c r="D22">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>1246</v>
       </c>
       <c r="E22">
         <f>10*$F$2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>5302.25</v>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>12460.25</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>623</v>
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>1246</v>
       </c>
       <c r="E23">
         <f t="shared" ref="E23:E25" si="5">10*$F$2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>5302.25</v>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>12460.25</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>623</v>
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>1246</v>
       </c>
       <c r="E24">
         <f t="shared" si="5"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>5302.25</v>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>12460.25</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>623</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>530</v>
+        <v>1246</v>
       </c>
       <c r="E25">
         <f t="shared" si="5"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>7391</v>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>33464.25</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>335</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>1673</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>739</v>
+        <v>3346</v>
       </c>
       <c r="E26">
         <f>15*$F$2</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>7391</v>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>33464.25</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>335</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>1673</v>
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>739</v>
+        <v>3346</v>
       </c>
       <c r="E27">
         <f t="shared" ref="E27:E30" si="6">15*$F$2</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>7391</v>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>33464.25</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>335</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>1673</v>
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
-        <v>739</v>
+        <v>3346</v>
       </c>
       <c r="E28">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>7391</v>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>33464.25</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>335</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>1673</v>
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
-        <v>739</v>
+        <v>3346</v>
       </c>
       <c r="E29">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>8958.5</v>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>66297</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>663</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>448</v>
+        <v>3315</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>896</v>
+        <v>6630</v>
       </c>
       <c r="E30">
         <f t="shared" si="6"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>8958.5</v>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>66297</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>663</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>448</v>
+        <v>3315</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
-        <v>896</v>
+        <v>6630</v>
       </c>
       <c r="E31">
         <f t="shared" ref="E31:E48" si="7">0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>8958.5</v>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>66297</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>663</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>448</v>
+        <v>3315</v>
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
-        <v>896</v>
+        <v>6630</v>
       </c>
       <c r="E32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>8958.5</v>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>66297</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>663</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>448</v>
+        <v>3315</v>
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
-        <v>896</v>
+        <v>6630</v>
       </c>
       <c r="E33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>8686.75</v>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>52173</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>522</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>2609</v>
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
-        <v>869</v>
+        <v>5217</v>
       </c>
       <c r="E34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>8686.75</v>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>52173</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>522</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>2609</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
-        <v>869</v>
+        <v>5217</v>
       </c>
       <c r="E35">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>8686.75</v>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>52173</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>522</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>2609</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>869</v>
+        <v>5217</v>
       </c>
       <c r="E36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>8686.75</v>
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>52173</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>522</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>434</v>
+        <v>2609</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>869</v>
+        <v>5217</v>
       </c>
       <c r="E37">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>5978.5</v>
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>17376.5</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>299</v>
+        <v>869</v>
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>598</v>
+        <v>1738</v>
       </c>
       <c r="E38">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>5978.5</v>
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>17376.5</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>299</v>
+        <v>869</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>598</v>
+        <v>1738</v>
       </c>
       <c r="E39">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>5978.5</v>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>17376.5</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>299</v>
+        <v>869</v>
       </c>
       <c r="D40">
         <f t="shared" si="2"/>
-        <v>598</v>
+        <v>1738</v>
       </c>
       <c r="E40">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>5978.5</v>
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>17376.5</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>299</v>
+        <v>869</v>
       </c>
       <c r="D41">
         <f t="shared" si="2"/>
-        <v>598</v>
+        <v>1738</v>
       </c>
       <c r="E41">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>4593.75</v>
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>7898</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>395</v>
       </c>
       <c r="D42">
         <f t="shared" si="2"/>
-        <v>459</v>
+        <v>790</v>
       </c>
       <c r="E42">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>4593.75</v>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>7898</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>395</v>
       </c>
       <c r="D43">
         <f t="shared" si="2"/>
-        <v>459</v>
+        <v>790</v>
       </c>
       <c r="E43">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>4593.75</v>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>7898</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>395</v>
       </c>
       <c r="D44">
         <f t="shared" si="2"/>
-        <v>459</v>
+        <v>790</v>
       </c>
       <c r="E44">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>4593.75</v>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>7898</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>395</v>
       </c>
       <c r="D45">
         <f t="shared" si="2"/>
-        <v>459</v>
+        <v>790</v>
       </c>
       <c r="E45">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>3860.5</v>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>5980.25</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>299</v>
       </c>
       <c r="D46">
         <f t="shared" si="2"/>
-        <v>386</v>
+        <v>598</v>
       </c>
       <c r="E46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>3860.5</v>
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>5980.25</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>299</v>
       </c>
       <c r="D47">
         <f t="shared" si="2"/>
-        <v>386</v>
+        <v>598</v>
       </c>
       <c r="E47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>3860.5</v>
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>5980.25</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>299</v>
       </c>
       <c r="D48">
         <f t="shared" si="2"/>
-        <v>386</v>
+        <v>598</v>
       </c>
       <c r="E48">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>3860.5</v>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>5980.25</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>299</v>
       </c>
       <c r="D49">
         <f t="shared" si="2"/>
-        <v>386</v>
+        <v>598</v>
       </c>
       <c r="E49">
         <f>2*$F$2</f>
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>3760.5</v>
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>25595</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>256</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>1280</v>
       </c>
       <c r="D50">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>2560</v>
       </c>
       <c r="E50">
         <f t="shared" ref="E50:E51" si="8">2*$F$2</f>
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>3760.5</v>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>25595</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>256</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>1280</v>
       </c>
       <c r="D51">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>2560</v>
       </c>
       <c r="E51">
         <f t="shared" si="8"/>
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>3760.5</v>
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>25595</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>256</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>1280</v>
       </c>
       <c r="D52">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>2560</v>
       </c>
       <c r="E52">
         <f>10*$F$2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>3760.5</v>
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>25595</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>256</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>188</v>
+        <v>1280</v>
       </c>
       <c r="D53">
         <f t="shared" si="2"/>
-        <v>376</v>
+        <v>2560</v>
       </c>
       <c r="E53">
         <f t="shared" ref="E53:E55" si="9">10*$F$2</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>3817</v>
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>26476</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>265</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>1324</v>
       </c>
       <c r="D54">
         <f t="shared" si="2"/>
-        <v>382</v>
+        <v>2648</v>
       </c>
       <c r="E54">
         <f t="shared" si="9"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>3817</v>
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>26476</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>265</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>1324</v>
       </c>
       <c r="D55">
         <f t="shared" si="2"/>
-        <v>382</v>
+        <v>2648</v>
       </c>
       <c r="E55">
         <f t="shared" si="9"/>
         <v>1000</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>3817</v>
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>26476</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>265</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>1324</v>
       </c>
       <c r="D56">
         <f t="shared" si="2"/>
-        <v>382</v>
+        <v>2648</v>
       </c>
       <c r="E56">
         <f>15*$F$2</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>3817</v>
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>26476</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>265</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>1324</v>
       </c>
       <c r="D57">
         <f t="shared" si="2"/>
-        <v>382</v>
+        <v>2648</v>
       </c>
       <c r="E57">
         <f t="shared" ref="E57:E60" si="10">15*$F$2</f>
         <v>1500</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>3455.25</v>
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>30789.25</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>1539</v>
       </c>
       <c r="D58">
         <f t="shared" si="2"/>
-        <v>346</v>
+        <v>3079</v>
       </c>
       <c r="E58">
         <f t="shared" si="10"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>3455.25</v>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>30789.25</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>1539</v>
       </c>
       <c r="D59">
         <f t="shared" si="2"/>
-        <v>346</v>
+        <v>3079</v>
       </c>
       <c r="E59">
         <f t="shared" si="10"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>3455.25</v>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>30789.25</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>1539</v>
       </c>
       <c r="D60">
         <f t="shared" si="2"/>
-        <v>346</v>
+        <v>3079</v>
       </c>
       <c r="E60">
         <f t="shared" si="10"/>
         <v>1500</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>3455.25</v>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
+        <v>30789.25</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>1539</v>
       </c>
       <c r="D61">
         <f t="shared" si="2"/>
-        <v>346</v>
+        <v>3079</v>
       </c>
       <c r="E61">
         <f>2*$F$2</f>
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>2811.75</v>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>44572.75</v>
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>446</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>2229</v>
       </c>
       <c r="D62">
         <f t="shared" si="2"/>
-        <v>281</v>
+        <v>4457</v>
       </c>
       <c r="E62">
         <f>1*$F$2</f>
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>2811.75</v>
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <v>44572.75</v>
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>446</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>2229</v>
       </c>
       <c r="D63">
         <f t="shared" si="2"/>
-        <v>281</v>
+        <v>4457</v>
       </c>
       <c r="E63">
         <f t="shared" ref="E63:E71" si="11">0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>2811.75</v>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>44572.75</v>
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>446</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>2229</v>
       </c>
       <c r="D64">
         <f t="shared" si="2"/>
-        <v>281</v>
+        <v>4457</v>
       </c>
       <c r="E64">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>2811.75</v>
+    <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <v>44572.75</v>
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>446</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>2229</v>
       </c>
       <c r="D65">
         <f t="shared" si="2"/>
-        <v>281</v>
+        <v>4457</v>
       </c>
       <c r="E65">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>2179.25</v>
+    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>56643</v>
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>566</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>2832</v>
       </c>
       <c r="D66">
         <f t="shared" si="2"/>
-        <v>218</v>
+        <v>5664</v>
       </c>
       <c r="E66">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>2179.25</v>
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <v>56643</v>
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B97" si="12">ROUND(A67*0.01,0)</f>
-        <v>22</v>
+        <v>566</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C97" si="13">ROUND(A67*0.05,0)</f>
-        <v>109</v>
+        <v>2832</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D97" si="14">ROUND(A67*0.1,0)</f>
-        <v>218</v>
+        <v>5664</v>
       </c>
       <c r="E67">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>2179.25</v>
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>56643</v>
       </c>
       <c r="B68">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>566</v>
       </c>
       <c r="C68">
         <f t="shared" si="13"/>
-        <v>109</v>
+        <v>2832</v>
       </c>
       <c r="D68">
         <f t="shared" si="14"/>
-        <v>218</v>
+        <v>5664</v>
       </c>
       <c r="E68">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>2179.25</v>
+    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>56643</v>
       </c>
       <c r="B69">
         <f t="shared" si="12"/>
-        <v>22</v>
+        <v>566</v>
       </c>
       <c r="C69">
         <f t="shared" si="13"/>
-        <v>109</v>
+        <v>2832</v>
       </c>
       <c r="D69">
         <f t="shared" si="14"/>
-        <v>218</v>
+        <v>5664</v>
       </c>
       <c r="E69">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>1525.25</v>
+    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <v>49975.25</v>
       </c>
       <c r="B70">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>500</v>
       </c>
       <c r="C70">
         <f t="shared" si="13"/>
-        <v>76</v>
+        <v>2499</v>
       </c>
       <c r="D70">
         <f t="shared" si="14"/>
-        <v>153</v>
+        <v>4998</v>
       </c>
       <c r="E70">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>1525.25</v>
+    <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>49975.25</v>
       </c>
       <c r="B71">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>500</v>
       </c>
       <c r="C71">
         <f t="shared" si="13"/>
-        <v>76</v>
+        <v>2499</v>
       </c>
       <c r="D71">
         <f t="shared" si="14"/>
-        <v>153</v>
+        <v>4998</v>
       </c>
       <c r="E71">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>1525.25</v>
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>49975.25</v>
       </c>
       <c r="B72">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>500</v>
       </c>
       <c r="C72">
         <f t="shared" si="13"/>
-        <v>76</v>
+        <v>2499</v>
       </c>
       <c r="D72">
         <f t="shared" si="14"/>
-        <v>153</v>
+        <v>4998</v>
       </c>
       <c r="E72">
         <f>20*$F$2</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>1525.25</v>
+    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>49975.25</v>
       </c>
       <c r="B73">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>500</v>
       </c>
       <c r="C73">
         <f t="shared" si="13"/>
-        <v>76</v>
+        <v>2499</v>
       </c>
       <c r="D73">
         <f t="shared" si="14"/>
-        <v>153</v>
+        <v>4998</v>
       </c>
       <c r="E73">
         <f t="shared" ref="E73:E75" si="15">20*$F$2</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>1027.75</v>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>32104</v>
       </c>
       <c r="B74">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>321</v>
       </c>
       <c r="C74">
         <f t="shared" si="13"/>
-        <v>51</v>
+        <v>1605</v>
       </c>
       <c r="D74">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>3210</v>
       </c>
       <c r="E74">
         <f t="shared" si="15"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>1027.75</v>
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>32104</v>
       </c>
       <c r="B75">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>321</v>
       </c>
       <c r="C75">
         <f t="shared" si="13"/>
-        <v>51</v>
+        <v>1605</v>
       </c>
       <c r="D75">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>3210</v>
       </c>
       <c r="E75">
         <f t="shared" si="15"/>
         <v>2000</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>1027.75</v>
+    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>32104</v>
       </c>
       <c r="B76">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>321</v>
       </c>
       <c r="C76">
         <f t="shared" si="13"/>
-        <v>51</v>
+        <v>1605</v>
       </c>
       <c r="D76">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>3210</v>
       </c>
       <c r="E76">
         <f>8*$F$2</f>
         <v>800</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>1027.75</v>
+    <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>32104</v>
       </c>
       <c r="B77">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>321</v>
       </c>
       <c r="C77">
         <f t="shared" si="13"/>
-        <v>51</v>
+        <v>1605</v>
       </c>
       <c r="D77">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>3210</v>
       </c>
       <c r="E77">
         <f>7*$F$2</f>
         <v>700</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>535</v>
+    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>22266.75</v>
       </c>
       <c r="B78">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C78">
         <f t="shared" si="13"/>
-        <v>27</v>
+        <v>1113</v>
       </c>
       <c r="D78">
         <f t="shared" si="14"/>
-        <v>54</v>
+        <v>2227</v>
       </c>
       <c r="E78">
         <f>2*$F$2</f>
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>535</v>
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>22266.75</v>
       </c>
       <c r="B79">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C79">
         <f t="shared" si="13"/>
-        <v>27</v>
+        <v>1113</v>
       </c>
       <c r="D79">
         <f t="shared" si="14"/>
-        <v>54</v>
+        <v>2227</v>
       </c>
       <c r="E79">
         <f t="shared" ref="E79:E87" si="16">0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>535</v>
+    <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>22266.75</v>
       </c>
       <c r="B80">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C80">
         <f t="shared" si="13"/>
-        <v>27</v>
+        <v>1113</v>
       </c>
       <c r="D80">
         <f t="shared" si="14"/>
-        <v>54</v>
+        <v>2227</v>
       </c>
       <c r="E80">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>535</v>
+    <row r="81" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>22266.75</v>
       </c>
       <c r="B81">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C81">
         <f t="shared" si="13"/>
-        <v>27</v>
+        <v>1113</v>
       </c>
       <c r="D81">
         <f t="shared" si="14"/>
-        <v>54</v>
+        <v>2227</v>
       </c>
       <c r="E81">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>599.25</v>
+    <row r="82" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>16930.5</v>
       </c>
       <c r="B82">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C82">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>847</v>
       </c>
       <c r="D82">
         <f t="shared" si="14"/>
-        <v>60</v>
+        <v>1693</v>
       </c>
       <c r="E82">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>599.25</v>
+    <row r="83" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>16930.5</v>
       </c>
       <c r="B83">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C83">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>847</v>
       </c>
       <c r="D83">
         <f t="shared" si="14"/>
-        <v>60</v>
+        <v>1693</v>
       </c>
       <c r="E83">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>599.25</v>
+    <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>16930.5</v>
       </c>
       <c r="B84">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C84">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>847</v>
       </c>
       <c r="D84">
         <f t="shared" si="14"/>
-        <v>60</v>
+        <v>1693</v>
       </c>
       <c r="E84">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>599.25</v>
+    <row r="85" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>16930.5</v>
       </c>
       <c r="B85">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="C85">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>847</v>
       </c>
       <c r="D85">
         <f t="shared" si="14"/>
-        <v>60</v>
+        <v>1693</v>
       </c>
       <c r="E85">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>742</v>
+    <row r="86" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>13005.25</v>
       </c>
       <c r="B86">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="C86">
         <f t="shared" si="13"/>
-        <v>37</v>
+        <v>650</v>
       </c>
       <c r="D86">
         <f t="shared" si="14"/>
-        <v>74</v>
+        <v>1301</v>
       </c>
       <c r="E86">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>742</v>
+    <row r="87" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>13005.25</v>
       </c>
       <c r="B87">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="C87">
         <f t="shared" si="13"/>
-        <v>37</v>
+        <v>650</v>
       </c>
       <c r="D87">
         <f t="shared" si="14"/>
-        <v>74</v>
+        <v>1301</v>
       </c>
       <c r="E87">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>742</v>
+    <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>13005.25</v>
       </c>
       <c r="B88">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="C88">
         <f t="shared" si="13"/>
-        <v>37</v>
+        <v>650</v>
       </c>
       <c r="D88">
         <f t="shared" si="14"/>
-        <v>74</v>
+        <v>1301</v>
       </c>
       <c r="E88">
         <f>25*$F$2</f>
         <v>2500</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>742</v>
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>13005.25</v>
       </c>
       <c r="B89">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="C89">
         <f t="shared" si="13"/>
-        <v>37</v>
+        <v>650</v>
       </c>
       <c r="D89">
         <f t="shared" si="14"/>
-        <v>74</v>
+        <v>1301</v>
       </c>
       <c r="E89">
         <f t="shared" ref="E89:E92" si="17">25*$F$2</f>
         <v>2500</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>723.25</v>
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>8475</v>
       </c>
       <c r="B90">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C90">
         <f t="shared" si="13"/>
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="D90">
         <f t="shared" si="14"/>
-        <v>72</v>
+        <v>848</v>
       </c>
       <c r="E90">
         <f t="shared" si="17"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>723.25</v>
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>8475</v>
       </c>
       <c r="B91">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C91">
         <f t="shared" si="13"/>
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="D91">
         <f t="shared" si="14"/>
-        <v>72</v>
+        <v>848</v>
       </c>
       <c r="E91">
         <f t="shared" si="17"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>723.25</v>
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>8475</v>
       </c>
       <c r="B92">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C92">
         <f t="shared" si="13"/>
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="D92">
         <f t="shared" si="14"/>
-        <v>72</v>
+        <v>848</v>
       </c>
       <c r="E92">
         <f t="shared" si="17"/>
         <v>2500</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>723.25</v>
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>8475</v>
       </c>
       <c r="B93">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C93">
         <f t="shared" si="13"/>
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="D93">
         <f t="shared" si="14"/>
-        <v>72</v>
+        <v>848</v>
       </c>
       <c r="E93">
         <f>5*$F$2</f>
         <v>500</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>334.5</v>
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>4897</v>
       </c>
       <c r="B94">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C94">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="D94">
         <f t="shared" si="14"/>
-        <v>33</v>
+        <v>490</v>
       </c>
       <c r="E94">
         <f>2*$F$2</f>
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>334.5</v>
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>4897</v>
       </c>
       <c r="B95">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C95">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="D95">
         <f t="shared" si="14"/>
-        <v>33</v>
+        <v>490</v>
       </c>
       <c r="E95">
         <f>1*$F$2</f>
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>334.5</v>
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>4897</v>
       </c>
       <c r="B96">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C96">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="D96">
         <f t="shared" si="14"/>
-        <v>33</v>
+        <v>490</v>
       </c>
       <c r="E96">
         <f>0*$F$2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>334.5</v>
+    <row r="97" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>4897</v>
       </c>
       <c r="B97">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C97">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="D97">
         <f t="shared" si="14"/>
-        <v>33</v>
+        <v>490</v>
       </c>
       <c r="E97">
         <f>0*$F$2</f>
@@ -2481,9 +3634,20 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <f>SUM(A2:A97)</f>
+        <v>2128407</v>
+      </c>
+      <c r="C103">
+        <f>100-(((A103-5692)/A103)*100)</f>
+        <v>0.26743005449615964</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>